<commit_message>
Fix poster fit and modal centering
</commit_message>
<xml_diff>
--- a/공연목록_오픈예정.xlsx
+++ b/공연목록_오픈예정.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddobi\Desktop\show\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83080940-387C-42D5-A6BB-EE0BE81A1D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CF95CF-537C-432C-83EF-309B62F10F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="2070" windowWidth="28140" windowHeight="17310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10260" yWindow="1440" windowWidth="28140" windowHeight="17310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="201">
   <si>
     <t>오픈일시</t>
   </si>
@@ -541,13 +541,118 @@
   </si>
   <si>
     <t>https://ticketimage.interpark.com/Play/image/large/25/25018629_p.gif</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2026010119363007.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/Play/image/large/25/25018118_p.gif</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/20260102042315.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025121715070785.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2026010217252356.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025121719172777.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025122915001553.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025123014460535.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/Play/image/large/25/25015600_p.gif</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/20260102050313.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/Play/image/large/25/25013784_p.gif</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/Play/image/large/25/25014553_p.gif</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025123015211549.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025123119191778.jpg</t>
+  </si>
+  <si>
+    <t>https://ticketimage.interpark.com/TicketImage/notice_poster/20/2025121715100246.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25018694_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025123113074940.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025123113173748.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25015215_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25017744_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025122620311357.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025122415045682.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25014944_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25015110_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025122619430664.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25015528_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025122621073344.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/25017505_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025122622183998.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%95_files/2025123020465677.jpg</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%9511_files/25018679_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%9511_files/25018649_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%9511_files/25015463_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%9511_files/25018356_p.gif</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ddobi/Desktop/show/images/NOL%20%ED%8B%B0%EC%BC%93%20_%20%EC%98%A4%ED%94%88%EC%98%88%EC%A0%9511_files/25018597_p.gif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,6 +676,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -614,15 +728,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -929,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -941,7 +1055,7 @@
     <col min="4" max="4" width="30.75" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
     <col min="6" max="6" width="54.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="66.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.25" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -986,6 +1100,9 @@
       <c r="F2" t="s">
         <v>119</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1006,6 +1123,9 @@
       <c r="F3" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1026,6 +1146,9 @@
       <c r="F4" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1046,6 +1169,9 @@
       <c r="F5" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1066,6 +1192,9 @@
       <c r="F6" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1086,6 +1215,9 @@
       <c r="F7" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="G7" s="2" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1106,6 +1238,9 @@
       <c r="F8" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="G8" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1126,6 +1261,9 @@
       <c r="F9" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1146,6 +1284,9 @@
       <c r="F10" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1166,6 +1307,9 @@
       <c r="F11" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1186,6 +1330,9 @@
       <c r="F12" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1206,6 +1353,9 @@
       <c r="F13" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="G13" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1226,6 +1376,9 @@
       <c r="F14" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="G14" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1246,6 +1399,9 @@
       <c r="F15" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1266,6 +1422,9 @@
       <c r="F16" t="s">
         <v>131</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1286,6 +1445,9 @@
       <c r="F17" t="s">
         <v>133</v>
       </c>
+      <c r="G17" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1306,6 +1468,9 @@
       <c r="F18" t="s">
         <v>134</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1326,6 +1491,9 @@
       <c r="F19" t="s">
         <v>135</v>
       </c>
+      <c r="G19" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1346,6 +1514,9 @@
       <c r="F20" t="s">
         <v>136</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1366,6 +1537,9 @@
       <c r="F21" t="s">
         <v>137</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1386,7 +1560,7 @@
       <c r="F22" t="s">
         <v>138</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1409,7 +1583,7 @@
       <c r="F23" t="s">
         <v>139</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="2" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1432,7 +1606,7 @@
       <c r="F24" t="s">
         <v>140</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1455,7 +1629,7 @@
       <c r="F25" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1478,6 +1652,9 @@
       <c r="F26" t="s">
         <v>142</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1498,6 +1675,9 @@
       <c r="F27" t="s">
         <v>143</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1518,6 +1698,9 @@
       <c r="F28" t="s">
         <v>144</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1538,6 +1721,9 @@
       <c r="F29" t="s">
         <v>145</v>
       </c>
+      <c r="G29" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1558,6 +1744,9 @@
       <c r="F30" t="s">
         <v>146</v>
       </c>
+      <c r="G30" s="2" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1578,6 +1767,9 @@
       <c r="F31" t="s">
         <v>147</v>
       </c>
+      <c r="G31" s="2" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1598,8 +1790,11 @@
       <c r="F32" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1618,8 +1813,11 @@
       <c r="F33" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1638,8 +1836,11 @@
       <c r="F34" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1658,8 +1859,11 @@
       <c r="F35" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1678,8 +1882,11 @@
       <c r="F36" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1698,8 +1905,11 @@
       <c r="F37" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1718,8 +1928,11 @@
       <c r="F38" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1738,8 +1951,11 @@
       <c r="F39" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -1758,10 +1974,13 @@
       <c r="F40" t="s">
         <v>156</v>
       </c>
+      <c r="G40" s="2" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="장르 선택" prompt="목록에서 장르를 선택해주세요." sqref="E2:E40" xr:uid="{A5C99B58-07E2-4CB5-8565-114A55B003D2}">
       <formula1>"콘서트,뮤지컬,연극,클래식,행사(전시),가족"</formula1>
     </dataValidation>

</xml_diff>